<commit_message>
Atualizado via W11: 2024-09-26.
</commit_message>
<xml_diff>
--- a/dados/avaliacao-chatgpt.xlsx
+++ b/dados/avaliacao-chatgpt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaopedroalbino/Downloads/GitHub/avaliacao-chatgpt/dados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\avaliacao-chatgpt\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72202EB-CCC3-C840-9298-7263FBE18F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28626386-5E68-45E6-92BC-BE1AD7C9B455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32840" yWindow="920" windowWidth="31040" windowHeight="17420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="20256" windowHeight="9720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respostas ao formulário 1" sheetId="1" r:id="rId1"/>
@@ -5097,39 +5097,39 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" customWidth="1"/>
-    <col min="3" max="3" width="33.1640625" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="33.109375" customWidth="1"/>
     <col min="4" max="4" width="34.33203125" customWidth="1"/>
     <col min="5" max="5" width="54.33203125" customWidth="1"/>
     <col min="6" max="6" width="47.33203125" customWidth="1"/>
     <col min="7" max="7" width="63.6640625" customWidth="1"/>
-    <col min="8" max="8" width="124.83203125" customWidth="1"/>
-    <col min="9" max="9" width="154.1640625" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" customWidth="1"/>
+    <col min="8" max="8" width="124.77734375" customWidth="1"/>
+    <col min="9" max="9" width="154.109375" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" customWidth="1"/>
     <col min="11" max="11" width="27.33203125" customWidth="1"/>
-    <col min="12" max="12" width="20.1640625" customWidth="1"/>
+    <col min="12" max="12" width="20.109375" customWidth="1"/>
     <col min="13" max="13" width="9" customWidth="1"/>
     <col min="14" max="14" width="20.6640625" customWidth="1"/>
-    <col min="15" max="15" width="30.1640625" customWidth="1"/>
-    <col min="16" max="16" width="130.1640625" customWidth="1"/>
+    <col min="15" max="15" width="30.109375" customWidth="1"/>
+    <col min="16" max="16" width="130.109375" customWidth="1"/>
     <col min="17" max="17" width="9.6640625" customWidth="1"/>
     <col min="18" max="18" width="83" customWidth="1"/>
-    <col min="19" max="19" width="46.83203125" customWidth="1"/>
+    <col min="19" max="19" width="46.77734375" customWidth="1"/>
     <col min="20" max="20" width="74.33203125" customWidth="1"/>
-    <col min="21" max="21" width="98.5" customWidth="1"/>
-    <col min="22" max="22" width="18.83203125" customWidth="1"/>
-    <col min="23" max="23" width="85.1640625" customWidth="1"/>
-    <col min="24" max="25" width="18.83203125" customWidth="1"/>
-    <col min="26" max="26" width="103.83203125" customWidth="1"/>
+    <col min="21" max="21" width="98.44140625" customWidth="1"/>
+    <col min="22" max="22" width="18.77734375" customWidth="1"/>
+    <col min="23" max="23" width="85.109375" customWidth="1"/>
+    <col min="24" max="25" width="18.77734375" customWidth="1"/>
+    <col min="26" max="26" width="103.77734375" customWidth="1"/>
     <col min="27" max="27" width="78" customWidth="1"/>
-    <col min="28" max="33" width="18.83203125" customWidth="1"/>
+    <col min="28" max="33" width="18.77734375" customWidth="1"/>
     <col min="34" max="1020" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:33" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1505</v>
       </c>
@@ -5218,7 +5218,7 @@
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
     </row>
-    <row r="2" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>40</v>
       </c>
@@ -5528,7 +5528,7 @@
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
     </row>
-    <row r="6" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
@@ -5606,7 +5606,7 @@
       </c>
       <c r="AA6" s="3"/>
     </row>
-    <row r="7" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -5682,7 +5682,7 @@
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
     </row>
-    <row r="8" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
@@ -5762,7 +5762,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -5834,7 +5834,7 @@
       </c>
       <c r="AA9" s="3"/>
     </row>
-    <row r="10" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -5912,7 +5912,7 @@
       </c>
       <c r="AA10" s="3"/>
     </row>
-    <row r="11" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
@@ -5960,7 +5960,7 @@
       </c>
       <c r="AA11" s="3"/>
     </row>
-    <row r="12" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>96</v>
       </c>
@@ -6032,7 +6032,7 @@
       </c>
       <c r="AA12" s="3"/>
     </row>
-    <row r="13" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -6104,7 +6104,7 @@
       </c>
       <c r="AA13" s="3"/>
     </row>
-    <row r="14" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -6187,7 +6187,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -6259,7 +6259,7 @@
       </c>
       <c r="AA15" s="3"/>
     </row>
-    <row r="16" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>129</v>
       </c>
@@ -6310,7 +6310,7 @@
       </c>
       <c r="AA16" s="3"/>
     </row>
-    <row r="17" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -6386,7 +6386,7 @@
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
     </row>
-    <row r="18" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>96</v>
       </c>
@@ -6458,7 +6458,7 @@
       </c>
       <c r="AA18" s="3"/>
     </row>
-    <row r="19" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
@@ -6534,7 +6534,7 @@
       <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
     </row>
-    <row r="20" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
@@ -6584,7 +6584,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>160</v>
       </c>
@@ -6630,7 +6630,7 @@
       <c r="Z21" s="3"/>
       <c r="AA21" s="3"/>
     </row>
-    <row r="22" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -6708,7 +6708,7 @@
       </c>
       <c r="AA22" s="3"/>
     </row>
-    <row r="23" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>96</v>
       </c>
@@ -6775,7 +6775,7 @@
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
     </row>
-    <row r="24" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
@@ -6856,7 +6856,7 @@
       </c>
       <c r="AA24" s="3"/>
     </row>
-    <row r="25" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>96</v>
       </c>
@@ -6926,7 +6926,7 @@
       <c r="Z25" s="3"/>
       <c r="AA25" s="3"/>
     </row>
-    <row r="26" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
@@ -7009,7 +7009,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>160</v>
       </c>
@@ -7083,7 +7083,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>160</v>
       </c>
@@ -7134,7 +7134,7 @@
       </c>
       <c r="AA28" s="3"/>
     </row>
-    <row r="29" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>160</v>
       </c>
@@ -7185,7 +7185,7 @@
       </c>
       <c r="AA29" s="3"/>
     </row>
-    <row r="30" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -7257,7 +7257,7 @@
       </c>
       <c r="AA30" s="3"/>
     </row>
-    <row r="31" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -7340,7 +7340,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
@@ -7419,7 +7419,7 @@
       <c r="Z32" s="3"/>
       <c r="AA32" s="3"/>
     </row>
-    <row r="33" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>96</v>
       </c>
@@ -7491,7 +7491,7 @@
       </c>
       <c r="AA33" s="3"/>
     </row>
-    <row r="34" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
@@ -7572,7 +7572,7 @@
       </c>
       <c r="AA34" s="3"/>
     </row>
-    <row r="35" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
@@ -7620,7 +7620,7 @@
       </c>
       <c r="AA35" s="3"/>
     </row>
-    <row r="36" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>0</v>
       </c>
@@ -7700,7 +7700,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>160</v>
       </c>
@@ -7778,7 +7778,7 @@
       </c>
       <c r="AA37" s="3"/>
     </row>
-    <row r="38" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>0</v>
       </c>
@@ -7848,7 +7848,7 @@
       <c r="Z38" s="3"/>
       <c r="AA38" s="3"/>
     </row>
-    <row r="39" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>160</v>
       </c>
@@ -7901,7 +7901,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="40" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>287</v>
       </c>
@@ -7981,7 +7981,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>28</v>
       </c>
@@ -8031,7 +8031,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>96</v>
       </c>
@@ -8112,7 +8112,7 @@
       </c>
       <c r="AA42" s="3"/>
     </row>
-    <row r="43" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>96</v>
       </c>
@@ -8190,7 +8190,7 @@
       </c>
       <c r="AA43" s="3"/>
     </row>
-    <row r="44" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>28</v>
       </c>
@@ -8268,7 +8268,7 @@
       </c>
       <c r="AA44" s="3"/>
     </row>
-    <row r="45" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>96</v>
       </c>
@@ -8314,7 +8314,7 @@
       <c r="Z45" s="3"/>
       <c r="AA45" s="3"/>
     </row>
-    <row r="46" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>0</v>
       </c>
@@ -8392,7 +8392,7 @@
       </c>
       <c r="AA46" s="3"/>
     </row>
-    <row r="47" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>0</v>
       </c>
@@ -8473,7 +8473,7 @@
       </c>
       <c r="AA47" s="3"/>
     </row>
-    <row r="48" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>96</v>
       </c>
@@ -8551,7 +8551,7 @@
       </c>
       <c r="AA48" s="3"/>
     </row>
-    <row r="49" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>160</v>
       </c>
@@ -8601,7 +8601,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>0</v>
       </c>
@@ -8673,7 +8673,7 @@
       </c>
       <c r="AA50" s="3"/>
     </row>
-    <row r="51" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>28</v>
       </c>
@@ -8745,7 +8745,7 @@
       </c>
       <c r="AA51" s="3"/>
     </row>
-    <row r="52" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>28</v>
       </c>
@@ -8825,7 +8825,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="53" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>96</v>
       </c>
@@ -8897,7 +8897,7 @@
       </c>
       <c r="AA53" s="3"/>
     </row>
-    <row r="54" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>28</v>
       </c>
@@ -8971,7 +8971,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="55" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>129</v>
       </c>
@@ -9052,7 +9052,7 @@
       </c>
       <c r="AA55" s="3"/>
     </row>
-    <row r="56" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>129</v>
       </c>
@@ -9122,7 +9122,7 @@
       <c r="Z56" s="3"/>
       <c r="AA56" s="3"/>
     </row>
-    <row r="57" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>40</v>
       </c>
@@ -9194,7 +9194,7 @@
       </c>
       <c r="AA57" s="3"/>
     </row>
-    <row r="58" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>96</v>
       </c>
@@ -9266,7 +9266,7 @@
       </c>
       <c r="AA58" s="3"/>
     </row>
-    <row r="59" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>28</v>
       </c>
@@ -9336,7 +9336,7 @@
       <c r="Z59" s="3"/>
       <c r="AA59" s="3"/>
     </row>
-    <row r="60" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>160</v>
       </c>
@@ -9384,7 +9384,7 @@
       </c>
       <c r="AA60" s="3"/>
     </row>
-    <row r="61" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>28</v>
       </c>
@@ -9456,7 +9456,7 @@
       </c>
       <c r="AA61" s="3"/>
     </row>
-    <row r="62" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>160</v>
       </c>
@@ -9526,7 +9526,7 @@
       <c r="Z62" s="3"/>
       <c r="AA62" s="3"/>
     </row>
-    <row r="63" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>28</v>
       </c>
@@ -9596,7 +9596,7 @@
       <c r="Z63" s="3"/>
       <c r="AA63" s="3"/>
     </row>
-    <row r="64" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>129</v>
       </c>
@@ -9644,7 +9644,7 @@
       </c>
       <c r="AA64" s="3"/>
     </row>
-    <row r="65" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>160</v>
       </c>
@@ -9716,7 +9716,7 @@
       </c>
       <c r="AA65" s="3"/>
     </row>
-    <row r="66" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>160</v>
       </c>
@@ -9766,7 +9766,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="67" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>96</v>
       </c>
@@ -9849,7 +9849,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="68" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>28</v>
       </c>
@@ -9923,7 +9923,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="69" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>129</v>
       </c>
@@ -9997,7 +9997,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="70" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>0</v>
       </c>
@@ -10075,7 +10075,7 @@
       </c>
       <c r="AA70" s="3"/>
     </row>
-    <row r="71" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>160</v>
       </c>
@@ -10121,7 +10121,7 @@
       <c r="Z71" s="3"/>
       <c r="AA71" s="3"/>
     </row>
-    <row r="72" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>0</v>
       </c>
@@ -10167,7 +10167,7 @@
       <c r="Z72" s="3"/>
       <c r="AA72" s="3"/>
     </row>
-    <row r="73" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>0</v>
       </c>
@@ -10237,7 +10237,7 @@
       <c r="Z73" s="3"/>
       <c r="AA73" s="3"/>
     </row>
-    <row r="74" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>129</v>
       </c>
@@ -10288,7 +10288,7 @@
       </c>
       <c r="AA74" s="3"/>
     </row>
-    <row r="75" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>160</v>
       </c>
@@ -10341,7 +10341,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="76" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>160</v>
       </c>
@@ -10419,7 +10419,7 @@
       </c>
       <c r="AA76" s="3"/>
     </row>
-    <row r="77" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>40</v>
       </c>
@@ -10500,7 +10500,7 @@
       </c>
       <c r="AA77" s="3"/>
     </row>
-    <row r="78" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>96</v>
       </c>
@@ -10578,7 +10578,7 @@
       </c>
       <c r="AA78" s="3"/>
     </row>
-    <row r="79" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>40</v>
       </c>
@@ -10656,7 +10656,7 @@
       </c>
       <c r="AA79" s="3"/>
     </row>
-    <row r="80" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>129</v>
       </c>
@@ -10702,7 +10702,7 @@
       <c r="Z80" s="3"/>
       <c r="AA80" s="3"/>
     </row>
-    <row r="81" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>28</v>
       </c>
@@ -10782,7 +10782,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="82" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>0</v>
       </c>
@@ -10858,7 +10858,7 @@
       <c r="Z82" s="3"/>
       <c r="AA82" s="3"/>
     </row>
-    <row r="83" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>40</v>
       </c>
@@ -10939,7 +10939,7 @@
       </c>
       <c r="AA83" s="3"/>
     </row>
-    <row r="84" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>160</v>
       </c>
@@ -11015,7 +11015,7 @@
       <c r="Z84" s="3"/>
       <c r="AA84" s="3"/>
     </row>
-    <row r="85" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>28</v>
       </c>
@@ -11093,7 +11093,7 @@
       </c>
       <c r="AA85" s="3"/>
     </row>
-    <row r="86" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>129</v>
       </c>
@@ -11165,7 +11165,7 @@
       </c>
       <c r="AA86" s="3"/>
     </row>
-    <row r="87" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>160</v>
       </c>
@@ -11213,7 +11213,7 @@
       </c>
       <c r="AA87" s="3"/>
     </row>
-    <row r="88" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>0</v>
       </c>
@@ -11283,7 +11283,7 @@
       <c r="Z88" s="3"/>
       <c r="AA88" s="3"/>
     </row>
-    <row r="89" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>28</v>
       </c>
@@ -11334,7 +11334,7 @@
       </c>
       <c r="AA89" s="3"/>
     </row>
-    <row r="90" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>96</v>
       </c>
@@ -11417,7 +11417,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="91" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>28</v>
       </c>
@@ -11487,7 +11487,7 @@
       <c r="Z91" s="3"/>
       <c r="AA91" s="3"/>
     </row>
-    <row r="92" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>0</v>
       </c>
@@ -11566,7 +11566,7 @@
       <c r="Z92" s="3"/>
       <c r="AA92" s="3"/>
     </row>
-    <row r="93" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>129</v>
       </c>
@@ -11647,7 +11647,7 @@
       </c>
       <c r="AA93" s="3"/>
     </row>
-    <row r="94" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>160</v>
       </c>
@@ -11697,7 +11697,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="95" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>0</v>
       </c>
@@ -11775,7 +11775,7 @@
       </c>
       <c r="AA95" s="3"/>
     </row>
-    <row r="96" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>28</v>
       </c>
@@ -11821,7 +11821,7 @@
       <c r="Z96" s="3"/>
       <c r="AA96" s="3"/>
     </row>
-    <row r="97" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>96</v>
       </c>
@@ -11864,7 +11864,7 @@
       <c r="Z97" s="3"/>
       <c r="AA97" s="3"/>
     </row>
-    <row r="98" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>0</v>
       </c>
@@ -11945,7 +11945,7 @@
       </c>
       <c r="AA98" s="3"/>
     </row>
-    <row r="99" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>0</v>
       </c>
@@ -12017,7 +12017,7 @@
       </c>
       <c r="AA99" s="3"/>
     </row>
-    <row r="100" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>129</v>
       </c>
@@ -12098,7 +12098,7 @@
       </c>
       <c r="AA100" s="3"/>
     </row>
-    <row r="101" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>160</v>
       </c>
@@ -12170,7 +12170,7 @@
       </c>
       <c r="AA101" s="3"/>
     </row>
-    <row r="102" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>129</v>
       </c>
@@ -12253,7 +12253,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="103" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>0</v>
       </c>
@@ -12336,7 +12336,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="104" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>28</v>
       </c>
@@ -12384,7 +12384,7 @@
       </c>
       <c r="AA104" s="3"/>
     </row>
-    <row r="105" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>160</v>
       </c>
@@ -12463,7 +12463,7 @@
       <c r="Z105" s="3"/>
       <c r="AA105" s="3"/>
     </row>
-    <row r="106" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>28</v>
       </c>
@@ -12544,7 +12544,7 @@
       </c>
       <c r="AA106" s="3"/>
     </row>
-    <row r="107" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>0</v>
       </c>
@@ -12625,7 +12625,7 @@
       </c>
       <c r="AA107" s="3"/>
     </row>
-    <row r="108" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>0</v>
       </c>
@@ -12671,7 +12671,7 @@
       <c r="Z108" s="3"/>
       <c r="AA108" s="3"/>
     </row>
-    <row r="109" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>129</v>
       </c>
@@ -12747,7 +12747,7 @@
       <c r="Z109" s="3"/>
       <c r="AA109" s="3"/>
     </row>
-    <row r="110" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>0</v>
       </c>
@@ -12795,7 +12795,7 @@
       </c>
       <c r="AA110" s="3"/>
     </row>
-    <row r="111" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>0</v>
       </c>
@@ -12843,7 +12843,7 @@
       </c>
       <c r="AA111" s="3"/>
     </row>
-    <row r="112" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>129</v>
       </c>
@@ -12921,7 +12921,7 @@
       </c>
       <c r="AA112" s="3"/>
     </row>
-    <row r="113" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>0</v>
       </c>
@@ -12997,7 +12997,7 @@
       <c r="Z113" s="3"/>
       <c r="AA113" s="3"/>
     </row>
-    <row r="114" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>96</v>
       </c>
@@ -13080,7 +13080,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="115" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>40</v>
       </c>
@@ -13159,7 +13159,7 @@
       <c r="Z115" s="3"/>
       <c r="AA115" s="3"/>
     </row>
-    <row r="116" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>96</v>
       </c>
@@ -13237,7 +13237,7 @@
       </c>
       <c r="AA116" s="3"/>
     </row>
-    <row r="117" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>0</v>
       </c>
@@ -13320,7 +13320,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="118" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>0</v>
       </c>
@@ -13396,7 +13396,7 @@
       <c r="Z118" s="3"/>
       <c r="AA118" s="3"/>
     </row>
-    <row r="119" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>96</v>
       </c>
@@ -13479,7 +13479,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="120" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>160</v>
       </c>
@@ -13562,7 +13562,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="121" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>129</v>
       </c>
@@ -13637,7 +13637,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="122" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>129</v>
       </c>
@@ -13718,7 +13718,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="123" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>28</v>
       </c>
@@ -13764,7 +13764,7 @@
       <c r="Z123" s="3"/>
       <c r="AA123" s="3"/>
     </row>
-    <row r="124" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>28</v>
       </c>
@@ -13840,7 +13840,7 @@
       <c r="Z124" s="3"/>
       <c r="AA124" s="3"/>
     </row>
-    <row r="125" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>96</v>
       </c>
@@ -13913,7 +13913,7 @@
       </c>
       <c r="AA125" s="3"/>
     </row>
-    <row r="126" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>0</v>
       </c>
@@ -13986,7 +13986,7 @@
       </c>
       <c r="AA126" s="3"/>
     </row>
-    <row r="127" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>40</v>
       </c>
@@ -14062,7 +14062,7 @@
       <c r="Z127" s="3"/>
       <c r="AA127" s="3"/>
     </row>
-    <row r="128" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>28</v>
       </c>
@@ -14140,7 +14140,7 @@
       </c>
       <c r="AA128" s="3"/>
     </row>
-    <row r="129" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>0</v>
       </c>
@@ -14218,7 +14218,7 @@
       </c>
       <c r="AA129" s="3"/>
     </row>
-    <row r="130" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>0</v>
       </c>
@@ -14291,7 +14291,7 @@
       </c>
       <c r="AA130" s="3"/>
     </row>
-    <row r="131" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>160</v>
       </c>
@@ -14337,7 +14337,7 @@
       <c r="Z131" s="3"/>
       <c r="AA131" s="3"/>
     </row>
-    <row r="132" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>160</v>
       </c>
@@ -14385,7 +14385,7 @@
       </c>
       <c r="AA132" s="3"/>
     </row>
-    <row r="133" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>160</v>
       </c>
@@ -14460,7 +14460,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="134" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>96</v>
       </c>
@@ -14541,7 +14541,7 @@
       </c>
       <c r="AA134" s="3"/>
     </row>
-    <row r="135" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>857</v>
       </c>
@@ -14617,7 +14617,7 @@
       <c r="Z135" s="3"/>
       <c r="AA135" s="3"/>
     </row>
-    <row r="136" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>28</v>
       </c>
@@ -14689,7 +14689,7 @@
       </c>
       <c r="AA136" s="3"/>
     </row>
-    <row r="137" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>160</v>
       </c>
@@ -14740,7 +14740,7 @@
       </c>
       <c r="AA137" s="3"/>
     </row>
-    <row r="138" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>160</v>
       </c>
@@ -14793,7 +14793,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="139" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>0</v>
       </c>
@@ -14869,7 +14869,7 @@
       <c r="Z139" s="3"/>
       <c r="AA139" s="3"/>
     </row>
-    <row r="140" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>96</v>
       </c>
@@ -14944,7 +14944,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="141" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>0</v>
       </c>
@@ -15027,7 +15027,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="142" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>40</v>
       </c>
@@ -15100,7 +15100,7 @@
       </c>
       <c r="AA142" s="3"/>
     </row>
-    <row r="143" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>0</v>
       </c>
@@ -15173,7 +15173,7 @@
       </c>
       <c r="AA143" s="3"/>
     </row>
-    <row r="144" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>160</v>
       </c>
@@ -15219,7 +15219,7 @@
       <c r="Z144" s="3"/>
       <c r="AA144" s="3"/>
     </row>
-    <row r="145" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>28</v>
       </c>
@@ -15302,7 +15302,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="146" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>96</v>
       </c>
@@ -15382,7 +15382,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="147" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>40</v>
       </c>
@@ -15455,7 +15455,7 @@
       </c>
       <c r="AA147" s="3"/>
     </row>
-    <row r="148" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>160</v>
       </c>
@@ -15501,7 +15501,7 @@
       <c r="Z148" s="3"/>
       <c r="AA148" s="3"/>
     </row>
-    <row r="149" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>0</v>
       </c>
@@ -15576,7 +15576,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="150" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>40</v>
       </c>
@@ -15652,7 +15652,7 @@
       <c r="Z150" s="3"/>
       <c r="AA150" s="3"/>
     </row>
-    <row r="151" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>40</v>
       </c>
@@ -15700,7 +15700,7 @@
       </c>
       <c r="AA151" s="3"/>
     </row>
-    <row r="152" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>40</v>
       </c>
@@ -15783,7 +15783,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="153" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>129</v>
       </c>
@@ -15861,7 +15861,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="154" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>40</v>
       </c>
@@ -15937,7 +15937,7 @@
       <c r="Z154" s="3"/>
       <c r="AA154" s="3"/>
     </row>
-    <row r="155" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>96</v>
       </c>
@@ -16018,7 +16018,7 @@
       </c>
       <c r="AA155" s="3"/>
     </row>
-    <row r="156" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>96</v>
       </c>
@@ -16091,7 +16091,7 @@
       </c>
       <c r="AA156" s="3"/>
     </row>
-    <row r="157" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>28</v>
       </c>
@@ -16169,7 +16169,7 @@
       </c>
       <c r="AA157" s="3"/>
     </row>
-    <row r="158" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>40</v>
       </c>
@@ -16244,7 +16244,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="159" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>129</v>
       </c>
@@ -16317,7 +16317,7 @@
       </c>
       <c r="AA159" s="3"/>
     </row>
-    <row r="160" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>40</v>
       </c>
@@ -16365,7 +16365,7 @@
       </c>
       <c r="AA160" s="3"/>
     </row>
-    <row r="161" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>160</v>
       </c>
@@ -16411,7 +16411,7 @@
       <c r="Z161" s="3"/>
       <c r="AA161" s="3"/>
     </row>
-    <row r="162" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>96</v>
       </c>
@@ -16494,7 +16494,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="163" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>0</v>
       </c>
@@ -16572,7 +16572,7 @@
       </c>
       <c r="AA163" s="3"/>
     </row>
-    <row r="164" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>96</v>
       </c>
@@ -16620,7 +16620,7 @@
       </c>
       <c r="AA164" s="3"/>
     </row>
-    <row r="165" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>28</v>
       </c>
@@ -16698,7 +16698,7 @@
       </c>
       <c r="AA165" s="3"/>
     </row>
-    <row r="166" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>160</v>
       </c>
@@ -16771,7 +16771,7 @@
       </c>
       <c r="AA166" s="3"/>
     </row>
-    <row r="167" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>160</v>
       </c>
@@ -16854,7 +16854,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="168" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>28</v>
       </c>
@@ -16935,7 +16935,7 @@
       </c>
       <c r="AA168" s="3"/>
     </row>
-    <row r="169" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>129</v>
       </c>
@@ -17016,7 +17016,7 @@
       </c>
       <c r="AA169" s="3"/>
     </row>
-    <row r="170" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>160</v>
       </c>
@@ -17067,7 +17067,7 @@
       </c>
       <c r="AA170" s="3"/>
     </row>
-    <row r="171" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>0</v>
       </c>
@@ -17138,7 +17138,7 @@
       <c r="Z171" s="3"/>
       <c r="AA171" s="3"/>
     </row>
-    <row r="172" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>160</v>
       </c>
@@ -17186,7 +17186,7 @@
       </c>
       <c r="AA172" s="3"/>
     </row>
-    <row r="173" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>0</v>
       </c>
@@ -17236,7 +17236,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="174" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>160</v>
       </c>
@@ -17286,7 +17286,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="175" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>160</v>
       </c>
@@ -17337,7 +17337,7 @@
       </c>
       <c r="AA175" s="3"/>
     </row>
-    <row r="176" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>0</v>
       </c>
@@ -17415,7 +17415,7 @@
       </c>
       <c r="AA176" s="3"/>
     </row>
-    <row r="177" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>28</v>
       </c>
@@ -17498,7 +17498,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="178" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>96</v>
       </c>
@@ -17574,7 +17574,7 @@
       <c r="Z178" s="3"/>
       <c r="AA178" s="3"/>
     </row>
-    <row r="179" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>857</v>
       </c>
@@ -17655,7 +17655,7 @@
       </c>
       <c r="AA179" s="3"/>
     </row>
-    <row r="180" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>160</v>
       </c>
@@ -17738,7 +17738,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="181" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>129</v>
       </c>
@@ -17814,7 +17814,7 @@
       <c r="Z181" s="3"/>
       <c r="AA181" s="3"/>
     </row>
-    <row r="182" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>160</v>
       </c>
@@ -17897,7 +17897,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="183" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>857</v>
       </c>
@@ -17975,7 +17975,7 @@
       </c>
       <c r="AA183" s="3"/>
     </row>
-    <row r="184" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>160</v>
       </c>
@@ -18026,7 +18026,7 @@
       </c>
       <c r="AA184" s="3"/>
     </row>
-    <row r="185" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>857</v>
       </c>
@@ -18099,7 +18099,7 @@
       </c>
       <c r="AA185" s="3"/>
     </row>
-    <row r="186" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>28</v>
       </c>
@@ -18145,7 +18145,7 @@
       <c r="Z186" s="3"/>
       <c r="AA186" s="3"/>
     </row>
-    <row r="187" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>129</v>
       </c>
@@ -18221,7 +18221,7 @@
       <c r="Z187" s="3"/>
       <c r="AA187" s="3"/>
     </row>
-    <row r="188" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>857</v>
       </c>
@@ -18299,7 +18299,7 @@
       </c>
       <c r="AA188" s="3"/>
     </row>
-    <row r="189" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>28</v>
       </c>
@@ -18378,7 +18378,7 @@
       <c r="Z189" s="3"/>
       <c r="AA189" s="3"/>
     </row>
-    <row r="190" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>160</v>
       </c>
@@ -18457,7 +18457,7 @@
       <c r="Z190" s="3"/>
       <c r="AA190" s="3"/>
     </row>
-    <row r="191" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>96</v>
       </c>
@@ -18503,7 +18503,7 @@
       <c r="Z191" s="3"/>
       <c r="AA191" s="3"/>
     </row>
-    <row r="192" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>160</v>
       </c>
@@ -18551,7 +18551,7 @@
       </c>
       <c r="AA192" s="3"/>
     </row>
-    <row r="193" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>96</v>
       </c>
@@ -18597,7 +18597,7 @@
       <c r="Z193" s="3"/>
       <c r="AA193" s="3"/>
     </row>
-    <row r="194" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>857</v>
       </c>
@@ -18673,7 +18673,7 @@
       <c r="Z194" s="3"/>
       <c r="AA194" s="3"/>
     </row>
-    <row r="195" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>28</v>
       </c>
@@ -18719,7 +18719,7 @@
       <c r="Z195" s="3"/>
       <c r="AA195" s="3"/>
     </row>
-    <row r="196" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>160</v>
       </c>
@@ -18797,7 +18797,7 @@
       </c>
       <c r="AA196" s="3"/>
     </row>
-    <row r="197" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>28</v>
       </c>
@@ -18845,7 +18845,7 @@
       </c>
       <c r="AA197" s="3"/>
     </row>
-    <row r="198" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>160</v>
       </c>
@@ -18893,7 +18893,7 @@
       </c>
       <c r="AA198" s="3"/>
     </row>
-    <row r="199" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>129</v>
       </c>
@@ -18971,7 +18971,7 @@
       </c>
       <c r="AA199" s="3"/>
     </row>
-    <row r="200" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>857</v>
       </c>
@@ -19052,7 +19052,7 @@
       </c>
       <c r="AA200" s="3"/>
     </row>
-    <row r="201" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>1216</v>
       </c>
@@ -19130,7 +19130,7 @@
       </c>
       <c r="AA201" s="3"/>
     </row>
-    <row r="202" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>857</v>
       </c>
@@ -19206,7 +19206,7 @@
       <c r="Z202" s="3"/>
       <c r="AA202" s="3"/>
     </row>
-    <row r="203" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>160</v>
       </c>
@@ -19259,7 +19259,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="204" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>857</v>
       </c>
@@ -19342,7 +19342,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="205" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>96</v>
       </c>
@@ -19415,7 +19415,7 @@
       </c>
       <c r="AA205" s="3"/>
     </row>
-    <row r="206" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>28</v>
       </c>
@@ -19463,7 +19463,7 @@
       </c>
       <c r="AA206" s="3"/>
     </row>
-    <row r="207" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>96</v>
       </c>
@@ -19541,7 +19541,7 @@
       </c>
       <c r="AA207" s="3"/>
     </row>
-    <row r="208" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>1216</v>
       </c>
@@ -19614,7 +19614,7 @@
       </c>
       <c r="AA208" s="3"/>
     </row>
-    <row r="209" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>28</v>
       </c>
@@ -19660,7 +19660,7 @@
       <c r="Z209" s="3"/>
       <c r="AA209" s="3"/>
     </row>
-    <row r="210" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>96</v>
       </c>
@@ -19736,7 +19736,7 @@
       <c r="Z210" s="3"/>
       <c r="AA210" s="3"/>
     </row>
-    <row r="211" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>1216</v>
       </c>
@@ -19811,7 +19811,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="212" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>287</v>
       </c>
@@ -19889,7 +19889,7 @@
       </c>
       <c r="AA212" s="3"/>
     </row>
-    <row r="213" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>1285</v>
       </c>
@@ -19935,7 +19935,7 @@
       <c r="Z213" s="3"/>
       <c r="AA213" s="3"/>
     </row>
-    <row r="214" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>857</v>
       </c>
@@ -20013,7 +20013,7 @@
       </c>
       <c r="AA214" s="3"/>
     </row>
-    <row r="215" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>287</v>
       </c>
@@ -20091,7 +20091,7 @@
       </c>
       <c r="AA215" s="3"/>
     </row>
-    <row r="216" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>160</v>
       </c>
@@ -20139,7 +20139,7 @@
       </c>
       <c r="AA216" s="3"/>
     </row>
-    <row r="217" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>287</v>
       </c>
@@ -20222,7 +20222,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="218" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>160</v>
       </c>
@@ -20303,7 +20303,7 @@
       </c>
       <c r="AA218" s="3"/>
     </row>
-    <row r="219" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>1285</v>
       </c>
@@ -20378,7 +20378,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="220" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>857</v>
       </c>
@@ -20427,7 +20427,7 @@
       <c r="Z220" s="3"/>
       <c r="AA220" s="3"/>
     </row>
-    <row r="221" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>287</v>
       </c>
@@ -20503,7 +20503,7 @@
       <c r="Z221" s="3"/>
       <c r="AA221" s="3"/>
     </row>
-    <row r="222" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>1285</v>
       </c>
@@ -20579,7 +20579,7 @@
       <c r="Z222" s="3"/>
       <c r="AA222" s="3"/>
     </row>
-    <row r="223" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>287</v>
       </c>
@@ -20662,7 +20662,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="224" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>160</v>
       </c>
@@ -20708,7 +20708,7 @@
       <c r="Z224" s="3"/>
       <c r="AA224" s="3"/>
     </row>
-    <row r="225" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
         <v>857</v>
       </c>
@@ -20779,7 +20779,7 @@
       <c r="Z225" s="3"/>
       <c r="AA225" s="3"/>
     </row>
-    <row r="226" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>160</v>
       </c>
@@ -20827,7 +20827,7 @@
       </c>
       <c r="AA226" s="3"/>
     </row>
-    <row r="227" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>287</v>
       </c>
@@ -20878,7 +20878,7 @@
       </c>
       <c r="AA227" s="3"/>
     </row>
-    <row r="228" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>857</v>
       </c>
@@ -20956,7 +20956,7 @@
       </c>
       <c r="AA228" s="3"/>
     </row>
-    <row r="229" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>287</v>
       </c>
@@ -21032,7 +21032,7 @@
       <c r="Z229" s="3"/>
       <c r="AA229" s="3"/>
     </row>
-    <row r="230" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>160</v>
       </c>
@@ -21080,7 +21080,7 @@
       </c>
       <c r="AA230" s="3"/>
     </row>
-    <row r="231" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>1285</v>
       </c>
@@ -21128,7 +21128,7 @@
       </c>
       <c r="AA231" s="3"/>
     </row>
-    <row r="232" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>1285</v>
       </c>
@@ -21174,7 +21174,7 @@
       <c r="Z232" s="3"/>
       <c r="AA232" s="3"/>
     </row>
-    <row r="233" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>1389</v>
       </c>
@@ -21250,7 +21250,7 @@
       <c r="Z233" s="3"/>
       <c r="AA233" s="3"/>
     </row>
-    <row r="234" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>1389</v>
       </c>
@@ -21333,7 +21333,7 @@
         <v>1404</v>
       </c>
     </row>
-    <row r="235" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>1285</v>
       </c>
@@ -21409,7 +21409,7 @@
       <c r="Z235" s="3"/>
       <c r="AA235" s="3"/>
     </row>
-    <row r="236" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>1285</v>
       </c>
@@ -21455,7 +21455,7 @@
       <c r="Z236" s="3"/>
       <c r="AA236" s="3"/>
     </row>
-    <row r="237" spans="1:27" ht="15" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>160</v>
       </c>
@@ -21503,7 +21503,7 @@
       </c>
       <c r="AA237" s="3"/>
     </row>
-    <row r="238" spans="1:27" ht="15" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>160</v>
       </c>
@@ -21556,7 +21556,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="239" spans="1:27" ht="15" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>287</v>
       </c>
@@ -21604,7 +21604,7 @@
       </c>
       <c r="AA239" s="3"/>
     </row>
-    <row r="240" spans="1:27" ht="15" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>287</v>
       </c>
@@ -21677,7 +21677,7 @@
       </c>
       <c r="AA240" s="3"/>
     </row>
-    <row r="241" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>0</v>
       </c>
@@ -21751,7 +21751,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="242" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>129</v>
       </c>
@@ -21831,7 +21831,7 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="243" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>28</v>
       </c>
@@ -21914,7 +21914,7 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="244" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>129</v>
       </c>
@@ -21961,7 +21961,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="245" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>0</v>
       </c>
@@ -22029,7 +22029,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="246" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="246" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>0</v>
       </c>
@@ -22100,7 +22100,7 @@
         <v>1454</v>
       </c>
     </row>
-    <row r="247" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="247" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>129</v>
       </c>
@@ -22171,7 +22171,7 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="248" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="248" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>28</v>
       </c>
@@ -22254,7 +22254,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="249" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="249" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>28</v>
       </c>
@@ -22331,7 +22331,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="250" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="250" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>96</v>
       </c>
@@ -22414,7 +22414,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="251" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="251" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>0</v>
       </c>
@@ -22482,7 +22482,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="252" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="252" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>0</v>
       </c>
@@ -22559,7 +22559,7 @@
         <v>1491</v>
       </c>
     </row>
-    <row r="253" spans="1:27" ht="15" x14ac:dyDescent="0.15">
+    <row r="253" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>40</v>
       </c>
@@ -22607,7 +22607,7 @@
       </c>
       <c r="AA253" s="3"/>
     </row>
-    <row r="254" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="254" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>40</v>
       </c>
@@ -22675,7 +22675,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="255" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="255" spans="1:27" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>40</v>
       </c>
@@ -22749,502 +22749,502 @@
         <v>62</v>
       </c>
     </row>
-    <row r="256" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="256" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S256" s="2"/>
       <c r="Z256" s="3"/>
       <c r="AA256" s="3"/>
     </row>
-    <row r="257" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="257" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S257" s="2"/>
       <c r="Z257" s="3"/>
       <c r="AA257" s="3"/>
     </row>
-    <row r="258" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="258" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S258" s="2"/>
       <c r="Z258" s="3"/>
       <c r="AA258" s="3"/>
     </row>
-    <row r="259" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="259" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S259" s="2"/>
       <c r="Z259" s="3"/>
       <c r="AA259" s="3"/>
     </row>
-    <row r="260" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="260" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S260" s="2"/>
       <c r="Z260" s="3"/>
       <c r="AA260" s="3"/>
     </row>
-    <row r="261" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="261" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S261" s="2"/>
       <c r="Z261" s="3"/>
       <c r="AA261" s="3"/>
     </row>
-    <row r="262" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="262" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S262" s="2"/>
       <c r="Z262" s="3"/>
       <c r="AA262" s="3"/>
     </row>
-    <row r="263" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="263" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S263" s="2"/>
       <c r="Z263" s="3"/>
       <c r="AA263" s="3"/>
     </row>
-    <row r="264" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="264" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S264" s="2"/>
       <c r="Z264" s="3"/>
       <c r="AA264" s="3"/>
     </row>
-    <row r="265" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="265" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S265" s="2"/>
       <c r="Z265" s="3"/>
       <c r="AA265" s="3"/>
     </row>
-    <row r="266" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="266" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S266" s="2"/>
       <c r="Z266" s="3"/>
       <c r="AA266" s="3"/>
     </row>
-    <row r="267" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="267" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S267" s="2"/>
       <c r="Z267" s="3"/>
       <c r="AA267" s="3"/>
     </row>
-    <row r="268" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="268" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S268" s="2"/>
       <c r="Z268" s="3"/>
       <c r="AA268" s="3"/>
     </row>
-    <row r="269" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="269" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S269" s="2"/>
       <c r="Z269" s="3"/>
       <c r="AA269" s="3"/>
     </row>
-    <row r="270" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="270" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S270" s="2"/>
       <c r="Z270" s="3"/>
       <c r="AA270" s="3"/>
     </row>
-    <row r="271" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="271" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S271" s="2"/>
       <c r="Z271" s="3"/>
       <c r="AA271" s="3"/>
     </row>
-    <row r="272" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="272" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S272" s="2"/>
       <c r="Z272" s="3"/>
       <c r="AA272" s="3"/>
     </row>
-    <row r="273" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="273" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S273" s="2"/>
       <c r="Z273" s="3"/>
       <c r="AA273" s="3"/>
     </row>
-    <row r="274" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="274" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S274" s="2"/>
       <c r="Z274" s="3"/>
       <c r="AA274" s="3"/>
     </row>
-    <row r="275" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="275" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S275" s="2"/>
       <c r="Z275" s="3"/>
       <c r="AA275" s="3"/>
     </row>
-    <row r="276" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="276" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S276" s="2"/>
       <c r="Z276" s="3"/>
       <c r="AA276" s="3"/>
     </row>
-    <row r="277" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="277" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S277" s="2"/>
       <c r="Z277" s="3"/>
       <c r="AA277" s="3"/>
     </row>
-    <row r="278" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="278" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S278" s="2"/>
       <c r="Z278" s="3"/>
       <c r="AA278" s="3"/>
     </row>
-    <row r="279" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="279" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S279" s="2"/>
       <c r="Z279" s="3"/>
       <c r="AA279" s="3"/>
     </row>
-    <row r="280" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="280" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S280" s="2"/>
       <c r="Z280" s="3"/>
       <c r="AA280" s="3"/>
     </row>
-    <row r="281" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="281" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S281" s="2"/>
       <c r="Z281" s="3"/>
       <c r="AA281" s="3"/>
     </row>
-    <row r="282" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="282" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S282" s="2"/>
       <c r="Z282" s="3"/>
       <c r="AA282" s="3"/>
     </row>
-    <row r="283" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="283" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S283" s="2"/>
       <c r="Z283" s="3"/>
       <c r="AA283" s="3"/>
     </row>
-    <row r="284" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="284" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S284" s="2"/>
       <c r="Z284" s="3"/>
       <c r="AA284" s="3"/>
     </row>
-    <row r="285" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="285" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S285" s="2"/>
       <c r="Z285" s="3"/>
       <c r="AA285" s="3"/>
     </row>
-    <row r="286" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="286" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S286" s="2"/>
       <c r="Z286" s="3"/>
       <c r="AA286" s="3"/>
     </row>
-    <row r="287" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="287" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S287" s="2"/>
       <c r="Z287" s="3"/>
       <c r="AA287" s="3"/>
     </row>
-    <row r="288" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="288" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S288" s="2"/>
       <c r="Z288" s="3"/>
       <c r="AA288" s="3"/>
     </row>
-    <row r="289" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="289" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S289" s="2"/>
       <c r="Z289" s="3"/>
       <c r="AA289" s="3"/>
     </row>
-    <row r="290" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="290" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S290" s="2"/>
       <c r="Z290" s="3"/>
       <c r="AA290" s="3"/>
     </row>
-    <row r="291" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="291" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S291" s="2"/>
       <c r="Z291" s="3"/>
       <c r="AA291" s="3"/>
     </row>
-    <row r="292" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="292" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S292" s="2"/>
       <c r="Z292" s="3"/>
       <c r="AA292" s="3"/>
     </row>
-    <row r="293" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="293" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S293" s="2"/>
       <c r="Z293" s="3"/>
       <c r="AA293" s="3"/>
     </row>
-    <row r="294" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="294" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S294" s="2"/>
       <c r="Z294" s="3"/>
       <c r="AA294" s="3"/>
     </row>
-    <row r="295" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="295" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S295" s="2"/>
       <c r="Z295" s="3"/>
       <c r="AA295" s="3"/>
     </row>
-    <row r="296" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="296" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S296" s="2"/>
       <c r="Z296" s="3"/>
       <c r="AA296" s="3"/>
     </row>
-    <row r="297" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="297" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S297" s="2"/>
       <c r="Z297" s="3"/>
       <c r="AA297" s="3"/>
     </row>
-    <row r="298" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="298" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S298" s="2"/>
       <c r="Z298" s="3"/>
       <c r="AA298" s="3"/>
     </row>
-    <row r="299" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="299" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S299" s="2"/>
       <c r="Z299" s="3"/>
       <c r="AA299" s="3"/>
     </row>
-    <row r="300" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="300" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S300" s="2"/>
       <c r="Z300" s="3"/>
       <c r="AA300" s="3"/>
     </row>
-    <row r="301" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="301" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S301" s="2"/>
       <c r="Z301" s="3"/>
       <c r="AA301" s="3"/>
     </row>
-    <row r="302" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="302" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S302" s="2"/>
       <c r="Z302" s="3"/>
       <c r="AA302" s="3"/>
     </row>
-    <row r="303" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="303" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S303" s="2"/>
       <c r="Z303" s="3"/>
       <c r="AA303" s="3"/>
     </row>
-    <row r="304" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="304" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S304" s="2"/>
       <c r="Z304" s="3"/>
       <c r="AA304" s="3"/>
     </row>
-    <row r="305" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="305" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S305" s="2"/>
       <c r="Z305" s="3"/>
       <c r="AA305" s="3"/>
     </row>
-    <row r="306" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="306" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S306" s="2"/>
       <c r="Z306" s="3"/>
       <c r="AA306" s="3"/>
     </row>
-    <row r="307" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="307" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S307" s="2"/>
       <c r="Z307" s="3"/>
       <c r="AA307" s="3"/>
     </row>
-    <row r="308" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="308" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S308" s="2"/>
       <c r="Z308" s="3"/>
       <c r="AA308" s="3"/>
     </row>
-    <row r="309" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="309" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S309" s="2"/>
       <c r="Z309" s="3"/>
       <c r="AA309" s="3"/>
     </row>
-    <row r="310" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="310" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S310" s="2"/>
       <c r="Z310" s="3"/>
       <c r="AA310" s="3"/>
     </row>
-    <row r="311" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="311" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S311" s="2"/>
       <c r="Z311" s="3"/>
       <c r="AA311" s="3"/>
     </row>
-    <row r="312" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="312" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S312" s="2"/>
       <c r="Z312" s="3"/>
       <c r="AA312" s="3"/>
     </row>
-    <row r="313" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="313" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S313" s="2"/>
       <c r="Z313" s="3"/>
       <c r="AA313" s="3"/>
     </row>
-    <row r="314" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="314" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S314" s="2"/>
       <c r="Z314" s="3"/>
       <c r="AA314" s="3"/>
     </row>
-    <row r="315" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="315" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S315" s="2"/>
       <c r="Z315" s="3"/>
       <c r="AA315" s="3"/>
     </row>
-    <row r="316" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="316" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S316" s="2"/>
       <c r="Z316" s="3"/>
       <c r="AA316" s="3"/>
     </row>
-    <row r="317" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="317" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S317" s="2"/>
       <c r="Z317" s="3"/>
       <c r="AA317" s="3"/>
     </row>
-    <row r="318" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="318" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S318" s="2"/>
       <c r="Z318" s="3"/>
       <c r="AA318" s="3"/>
     </row>
-    <row r="319" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="319" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S319" s="2"/>
       <c r="Z319" s="3"/>
       <c r="AA319" s="3"/>
     </row>
-    <row r="320" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="320" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S320" s="2"/>
       <c r="Z320" s="3"/>
       <c r="AA320" s="3"/>
     </row>
-    <row r="321" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="321" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S321" s="2"/>
       <c r="Z321" s="3"/>
       <c r="AA321" s="3"/>
     </row>
-    <row r="322" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="322" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S322" s="2"/>
       <c r="Z322" s="3"/>
       <c r="AA322" s="3"/>
     </row>
-    <row r="323" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="323" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S323" s="2"/>
       <c r="Z323" s="3"/>
       <c r="AA323" s="3"/>
     </row>
-    <row r="324" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="324" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S324" s="2"/>
       <c r="Z324" s="3"/>
       <c r="AA324" s="3"/>
     </row>
-    <row r="325" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="325" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S325" s="2"/>
       <c r="Z325" s="3"/>
       <c r="AA325" s="3"/>
     </row>
-    <row r="326" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="326" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S326" s="2"/>
       <c r="Z326" s="3"/>
       <c r="AA326" s="3"/>
     </row>
-    <row r="327" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="327" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S327" s="2"/>
       <c r="Z327" s="3"/>
       <c r="AA327" s="3"/>
     </row>
-    <row r="328" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="328" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S328" s="2"/>
       <c r="Z328" s="3"/>
       <c r="AA328" s="3"/>
     </row>
-    <row r="329" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="329" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S329" s="2"/>
       <c r="Z329" s="3"/>
       <c r="AA329" s="3"/>
     </row>
-    <row r="330" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="330" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S330" s="2"/>
       <c r="Z330" s="3"/>
       <c r="AA330" s="3"/>
     </row>
-    <row r="331" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="331" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S331" s="2"/>
       <c r="Z331" s="3"/>
       <c r="AA331" s="3"/>
     </row>
-    <row r="332" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="332" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S332" s="2"/>
       <c r="Z332" s="3"/>
       <c r="AA332" s="3"/>
     </row>
-    <row r="333" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="333" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S333" s="2"/>
       <c r="Z333" s="3"/>
       <c r="AA333" s="3"/>
     </row>
-    <row r="334" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="334" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S334" s="2"/>
       <c r="Z334" s="3"/>
       <c r="AA334" s="3"/>
     </row>
-    <row r="335" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="335" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S335" s="2"/>
       <c r="Z335" s="3"/>
       <c r="AA335" s="3"/>
     </row>
-    <row r="336" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="336" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S336" s="2"/>
       <c r="Z336" s="3"/>
       <c r="AA336" s="3"/>
     </row>
-    <row r="337" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="337" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S337" s="2"/>
       <c r="Z337" s="3"/>
       <c r="AA337" s="3"/>
     </row>
-    <row r="338" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="338" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S338" s="2"/>
       <c r="Z338" s="3"/>
       <c r="AA338" s="3"/>
     </row>
-    <row r="339" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="339" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S339" s="2"/>
       <c r="Z339" s="3"/>
       <c r="AA339" s="3"/>
     </row>
-    <row r="340" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="340" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S340" s="2"/>
       <c r="Z340" s="3"/>
       <c r="AA340" s="3"/>
     </row>
-    <row r="341" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="341" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S341" s="2"/>
       <c r="Z341" s="3"/>
       <c r="AA341" s="3"/>
     </row>
-    <row r="342" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="342" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S342" s="2"/>
       <c r="Z342" s="3"/>
       <c r="AA342" s="3"/>
     </row>
-    <row r="343" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="343" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S343" s="2"/>
       <c r="Z343" s="3"/>
       <c r="AA343" s="3"/>
     </row>
-    <row r="344" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="344" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S344" s="2"/>
       <c r="Z344" s="3"/>
       <c r="AA344" s="3"/>
     </row>
-    <row r="345" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="345" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S345" s="2"/>
       <c r="Z345" s="3"/>
       <c r="AA345" s="3"/>
     </row>
-    <row r="346" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="346" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S346" s="2"/>
       <c r="Z346" s="3"/>
       <c r="AA346" s="3"/>
     </row>
-    <row r="347" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="347" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S347" s="2"/>
       <c r="Z347" s="3"/>
       <c r="AA347" s="3"/>
     </row>
-    <row r="348" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="348" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S348" s="2"/>
       <c r="Z348" s="3"/>
       <c r="AA348" s="3"/>
     </row>
-    <row r="349" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="349" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S349" s="2"/>
       <c r="Z349" s="3"/>
       <c r="AA349" s="3"/>
     </row>
-    <row r="350" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="350" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S350" s="2"/>
       <c r="Z350" s="3"/>
       <c r="AA350" s="3"/>
     </row>
-    <row r="351" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="351" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S351" s="2"/>
       <c r="Z351" s="3"/>
       <c r="AA351" s="3"/>
     </row>
-    <row r="352" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="352" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S352" s="2"/>
       <c r="Z352" s="3"/>
       <c r="AA352" s="3"/>
     </row>
-    <row r="353" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="353" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S353" s="2"/>
       <c r="Z353" s="3"/>
       <c r="AA353" s="3"/>
     </row>
-    <row r="354" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="354" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S354" s="2"/>
       <c r="Z354" s="3"/>
       <c r="AA354" s="3"/>
     </row>
-    <row r="355" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="355" spans="19:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S355" s="2"/>
       <c r="Z355" s="3"/>
       <c r="AA355" s="3"/>

</xml_diff>

<commit_message>
Atualizando arquivos em OSx: 2024-09-30.
</commit_message>
<xml_diff>
--- a/dados/avaliacao-chatgpt.xlsx
+++ b/dados/avaliacao-chatgpt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaopedroalbino/Downloads/GitHub/avaliacao-chatgpt/dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72202EB-CCC3-C840-9298-7263FBE18F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3616E4BE-5A6C-7245-819F-E5F89790F639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32840" yWindow="920" windowWidth="31040" windowHeight="17420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32560" yWindow="1000" windowWidth="31040" windowHeight="17420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respostas ao formulário 1" sheetId="1" r:id="rId1"/>
@@ -5093,8 +5093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG355"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="P20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>